<commit_message>
rapport de stage à jour+ intégration partielle des données à la cvtech
</commit_message>
<xml_diff>
--- a/Projet_Matrice/Matrices/46.xlsx
+++ b/Projet_Matrice/Matrices/46.xlsx
@@ -881,7 +881,7 @@
     <t>Tech lead Java</t>
   </si>
   <si>
-    <t>Nom/Prénom  : CABY MAXIME</t>
+    <t xml:space="preserve">Nom/Prénom  : MAXIME CABY </t>
   </si>
   <si>
     <t>Soft Skills</t>
@@ -1319,13 +1319,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1718,7 +1724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1726,8 +1732,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1735,22 +1741,22 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -1762,94 +1768,103 @@
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="13" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="14" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="12" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="13" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="14" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="13" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="15" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="16" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="14" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="15" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="16" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -2205,87 +2220,87 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="46" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="46" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="46" width="34.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="47" width="115.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="49" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="49" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="49" width="34.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="50" width="115.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="37"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="40"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="57.75">
-      <c r="A2" s="38">
+      <c r="A2" s="41">
         <f>("⭐")</f>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="42" t="s">
         <v>316</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="43" t="s">
         <v>317</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="44" t="s">
         <v>318</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="57.75">
-      <c r="A3" s="38">
+      <c r="A3" s="41">
         <f>("⭐⭐")</f>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>319</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="43" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="44" t="s">
         <v>321</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="57.75">
-      <c r="A4" s="38">
+      <c r="A4" s="41">
         <f>("⭐⭐⭐")</f>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="42" t="s">
         <v>322</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="43" t="s">
         <v>323</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="44" t="s">
         <v>324</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="57.75">
-      <c r="A5" s="38">
+      <c r="A5" s="41">
         <f>("⭐⭐⭐⭐")</f>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="42" t="s">
         <v>325</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="43" t="s">
         <v>326</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="44" t="s">
         <v>327</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="57.75">
-      <c r="A6" s="42">
+      <c r="A6" s="45">
         <f>("⭐⭐⭐⭐⭐")</f>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="46" t="s">
         <v>328</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="47" t="s">
         <v>329</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="48" t="s">
         <v>330</v>
       </c>
     </row>
@@ -2308,19 +2323,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="34" width="64.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="36" width="64.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="37" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="4" width="25.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>308</v>
       </c>
       <c r="B1" s="1"/>
@@ -2328,84 +2343,84 @@
       <c r="D1" s="1"/>
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="3"/>
       <c r="I1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="52.5" customFormat="1" s="26">
-      <c r="A2" s="27" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="52.5" customFormat="1" s="28">
+      <c r="A2" s="29" t="s">
         <v>309</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="28"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="78" customFormat="1" s="26">
-      <c r="A3" s="27" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="30"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="78" customFormat="1" s="28">
+      <c r="A3" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="30"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="64.5">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="29" t="s">
         <v>311</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="31">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33">
         <v>1</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="34">
         <f>REPT("⭐",E4)</f>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="31">
+      <c r="G4" s="27"/>
+      <c r="H4" s="33">
         <v>4</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="34">
         <f>REPT("⭐",H4)</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="52.5" customFormat="1" s="26">
-      <c r="A5" s="27" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="52.5" customFormat="1" s="28">
+      <c r="A5" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="28"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="52.5" customFormat="1" s="26">
-      <c r="A6" s="33" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="30"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="52.5" customFormat="1" s="28">
+      <c r="A6" s="35" t="s">
         <v>314</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="28"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2452,719 +2467,719 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="24">
       <c r="A5" s="1"/>
-      <c r="B5" s="21"/>
+      <c r="B5" s="22"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="23" t="s">
         <v>285</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="23" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="23" t="s">
+      <c r="B7" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="23" t="s">
+      <c r="B8" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="23" t="s">
+      <c r="B9" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="24" t="s">
         <v>289</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="23" t="s">
+      <c r="B10" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="24" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="23" t="s">
+      <c r="B11" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="23" t="s">
+      <c r="B12" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="23" t="s">
+      <c r="B13" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="23" t="s">
+      <c r="B14" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="22.5">
-      <c r="A16" s="23" t="s">
+      <c r="B15" s="25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="24" t="s">
         <v>295</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="22.5">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="22.5">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="24" t="s">
         <v>297</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="22.5">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="22.5">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="24" t="s">
         <v>299</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="22.5">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="22.5">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="22.5">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="22.5">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="24" t="s">
         <v>303</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="22.5">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="24" t="s">
         <v>304</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="22.5">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="24" t="s">
         <v>305</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="22.5">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="24" t="s">
         <v>306</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="22.5">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="24" t="s">
         <v>307</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="22.5">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24" t="s">
+      <c r="A29" s="24"/>
+      <c r="B29" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="22.5">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24" t="s">
+      <c r="A30" s="24"/>
+      <c r="B30" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="22.5">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24" t="s">
+      <c r="A31" s="24"/>
+      <c r="B31" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="22.5">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24" t="s">
+      <c r="A32" s="24"/>
+      <c r="B32" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="22.5">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24" t="s">
+      <c r="A33" s="24"/>
+      <c r="B33" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="22.5">
-      <c r="A34" s="23"/>
-      <c r="B34" s="24" t="s">
+      <c r="A34" s="24"/>
+      <c r="B34" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="22.5">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24" t="s">
+      <c r="A35" s="24"/>
+      <c r="B35" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="22.5">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24" t="s">
+      <c r="A36" s="24"/>
+      <c r="B36" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="22.5">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24" t="s">
+      <c r="A37" s="24"/>
+      <c r="B37" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="22.5">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24" t="s">
+      <c r="A38" s="24"/>
+      <c r="B38" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="22.5">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24" t="s">
+      <c r="A39" s="24"/>
+      <c r="B39" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="22.5">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24" t="s">
+      <c r="A40" s="24"/>
+      <c r="B40" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="22.5">
-      <c r="A41" s="23"/>
-      <c r="B41" s="24" t="s">
+      <c r="A41" s="24"/>
+      <c r="B41" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="22.5">
-      <c r="A42" s="23"/>
-      <c r="B42" s="24" t="s">
+      <c r="A42" s="24"/>
+      <c r="B42" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="22.5">
       <c r="A43" s="1"/>
-      <c r="B43" s="24"/>
+      <c r="B43" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="22.5">
       <c r="A44" s="1"/>
-      <c r="B44" s="24"/>
+      <c r="B44" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="22.5">
       <c r="A45" s="1"/>
-      <c r="B45" s="24"/>
+      <c r="B45" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="22.5">
       <c r="A46" s="1"/>
-      <c r="B46" s="24"/>
+      <c r="B46" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="22.5">
       <c r="A47" s="1"/>
-      <c r="B47" s="24"/>
+      <c r="B47" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="22.5">
       <c r="A48" s="1"/>
-      <c r="B48" s="24"/>
+      <c r="B48" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="22.5">
       <c r="A49" s="1"/>
-      <c r="B49" s="24"/>
+      <c r="B49" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="22.5">
       <c r="A50" s="1"/>
-      <c r="B50" s="24"/>
+      <c r="B50" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="22.5">
       <c r="A51" s="1"/>
-      <c r="B51" s="24"/>
+      <c r="B51" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="22.5">
       <c r="A52" s="1"/>
-      <c r="B52" s="24"/>
+      <c r="B52" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="22.5">
       <c r="A53" s="1"/>
-      <c r="B53" s="24"/>
+      <c r="B53" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="22.5">
       <c r="A54" s="1"/>
-      <c r="B54" s="24"/>
+      <c r="B54" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="22.5">
       <c r="A55" s="1"/>
-      <c r="B55" s="24"/>
+      <c r="B55" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="22.5">
       <c r="A56" s="1"/>
-      <c r="B56" s="24"/>
+      <c r="B56" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="22.5">
       <c r="A57" s="1"/>
-      <c r="B57" s="24"/>
+      <c r="B57" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="22.5">
       <c r="A58" s="1"/>
-      <c r="B58" s="24"/>
+      <c r="B58" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="22.5">
       <c r="A59" s="1"/>
-      <c r="B59" s="24"/>
+      <c r="B59" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="22.5">
       <c r="A60" s="1"/>
-      <c r="B60" s="24"/>
+      <c r="B60" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="22.5">
       <c r="A61" s="1"/>
-      <c r="B61" s="24"/>
+      <c r="B61" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="22.5">
       <c r="A62" s="1"/>
-      <c r="B62" s="24"/>
+      <c r="B62" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="22.5">
       <c r="A63" s="1"/>
-      <c r="B63" s="24"/>
+      <c r="B63" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="22.5">
       <c r="A64" s="1"/>
-      <c r="B64" s="24"/>
+      <c r="B64" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="22.5">
       <c r="A65" s="1"/>
-      <c r="B65" s="24"/>
+      <c r="B65" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="22.5">
       <c r="A66" s="1"/>
-      <c r="B66" s="24"/>
+      <c r="B66" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="22.5">
       <c r="A67" s="1"/>
-      <c r="B67" s="24"/>
+      <c r="B67" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="22.5">
       <c r="A68" s="1"/>
-      <c r="B68" s="24"/>
+      <c r="B68" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="22.5">
       <c r="A69" s="1"/>
-      <c r="B69" s="24"/>
+      <c r="B69" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="22.5">
       <c r="A70" s="1"/>
-      <c r="B70" s="24"/>
+      <c r="B70" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="22.5">
       <c r="A71" s="1"/>
-      <c r="B71" s="24"/>
+      <c r="B71" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="22.5">
       <c r="A72" s="1"/>
-      <c r="B72" s="24"/>
+      <c r="B72" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="22.5">
       <c r="A73" s="1"/>
-      <c r="B73" s="24"/>
+      <c r="B73" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="22.5">
       <c r="A74" s="1"/>
-      <c r="B74" s="24"/>
+      <c r="B74" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="22.5">
       <c r="A75" s="1"/>
-      <c r="B75" s="24"/>
+      <c r="B75" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="22.5">
       <c r="A76" s="1"/>
-      <c r="B76" s="24"/>
+      <c r="B76" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="22.5">
       <c r="A77" s="1"/>
-      <c r="B77" s="24"/>
+      <c r="B77" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="22.5">
       <c r="A78" s="1"/>
-      <c r="B78" s="24"/>
+      <c r="B78" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="22.5">
       <c r="A79" s="1"/>
-      <c r="B79" s="24"/>
+      <c r="B79" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="22.5">
       <c r="A80" s="1"/>
-      <c r="B80" s="24"/>
+      <c r="B80" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="22.5">
       <c r="A81" s="1"/>
-      <c r="B81" s="24"/>
+      <c r="B81" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="22.5">
       <c r="A82" s="1"/>
-      <c r="B82" s="24"/>
+      <c r="B82" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="22.5">
       <c r="A83" s="1"/>
-      <c r="B83" s="24"/>
+      <c r="B83" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="22.5">
       <c r="A84" s="1"/>
-      <c r="B84" s="24"/>
+      <c r="B84" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="22.5">
       <c r="A85" s="1"/>
-      <c r="B85" s="24"/>
+      <c r="B85" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="22.5">
       <c r="A86" s="1"/>
-      <c r="B86" s="24"/>
+      <c r="B86" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="22.5">
       <c r="A87" s="1"/>
-      <c r="B87" s="24"/>
+      <c r="B87" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="22.5">
       <c r="A88" s="1"/>
-      <c r="B88" s="24"/>
+      <c r="B88" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="22.5">
       <c r="A89" s="1"/>
-      <c r="B89" s="24"/>
+      <c r="B89" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="22.5">
       <c r="A90" s="1"/>
-      <c r="B90" s="24"/>
+      <c r="B90" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="22.5">
       <c r="A91" s="1"/>
-      <c r="B91" s="24"/>
+      <c r="B91" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="22.5">
       <c r="A92" s="1"/>
-      <c r="B92" s="24"/>
+      <c r="B92" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="22.5">
       <c r="A93" s="1"/>
-      <c r="B93" s="24"/>
+      <c r="B93" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="22.5">
       <c r="A94" s="1"/>
-      <c r="B94" s="24"/>
+      <c r="B94" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="22.5">
       <c r="A95" s="1"/>
-      <c r="B95" s="24"/>
+      <c r="B95" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="22.5">
       <c r="A96" s="1"/>
-      <c r="B96" s="24"/>
+      <c r="B96" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="22.5">
       <c r="A97" s="1"/>
-      <c r="B97" s="24"/>
+      <c r="B97" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="22.5">
       <c r="A98" s="1"/>
-      <c r="B98" s="24"/>
+      <c r="B98" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="22.5">
       <c r="A99" s="1"/>
-      <c r="B99" s="24"/>
+      <c r="B99" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="22.5">
       <c r="A100" s="1"/>
-      <c r="B100" s="24"/>
+      <c r="B100" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="22.5">
       <c r="A101" s="1"/>
-      <c r="B101" s="24"/>
+      <c r="B101" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="22.5">
       <c r="A102" s="1"/>
-      <c r="B102" s="24"/>
+      <c r="B102" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="22.5">
       <c r="A103" s="1"/>
-      <c r="B103" s="24"/>
+      <c r="B103" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="22.5">
       <c r="A104" s="1"/>
-      <c r="B104" s="24"/>
+      <c r="B104" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="22.5">
       <c r="A105" s="1"/>
-      <c r="B105" s="24"/>
+      <c r="B105" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="22.5">
       <c r="A106" s="1"/>
-      <c r="B106" s="24"/>
+      <c r="B106" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="22.5">
       <c r="A107" s="1"/>
-      <c r="B107" s="24"/>
+      <c r="B107" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="22.5">
       <c r="A108" s="1"/>
-      <c r="B108" s="24"/>
+      <c r="B108" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="22.5">
       <c r="A109" s="1"/>
-      <c r="B109" s="24"/>
+      <c r="B109" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="22.5">
       <c r="A110" s="1"/>
-      <c r="B110" s="24"/>
+      <c r="B110" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="22.5">
       <c r="A111" s="1"/>
-      <c r="B111" s="24"/>
+      <c r="B111" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="22.5">
       <c r="A112" s="1"/>
-      <c r="B112" s="24"/>
+      <c r="B112" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="22.5">
       <c r="A113" s="1"/>
-      <c r="B113" s="24"/>
+      <c r="B113" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="22.5">
       <c r="A114" s="1"/>
-      <c r="B114" s="24"/>
+      <c r="B114" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="22.5">
       <c r="A115" s="1"/>
-      <c r="B115" s="24"/>
+      <c r="B115" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="22.5">
       <c r="A116" s="1"/>
-      <c r="B116" s="24"/>
+      <c r="B116" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="22.5">
       <c r="A117" s="1"/>
-      <c r="B117" s="24"/>
+      <c r="B117" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="22.5">
       <c r="A118" s="1"/>
-      <c r="B118" s="24"/>
+      <c r="B118" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="22.5">
       <c r="A119" s="1"/>
-      <c r="B119" s="24"/>
+      <c r="B119" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="22.5">
       <c r="A120" s="1"/>
-      <c r="B120" s="24"/>
+      <c r="B120" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="22.5">
       <c r="A121" s="1"/>
-      <c r="B121" s="24"/>
+      <c r="B121" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="22.5">
       <c r="A122" s="1"/>
-      <c r="B122" s="24"/>
+      <c r="B122" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="22.5">
       <c r="A123" s="1"/>
-      <c r="B123" s="24"/>
+      <c r="B123" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="22.5">
       <c r="A124" s="1"/>
-      <c r="B124" s="24"/>
+      <c r="B124" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="22.5">
       <c r="A125" s="1"/>
-      <c r="B125" s="24"/>
+      <c r="B125" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="22.5">
       <c r="A126" s="1"/>
-      <c r="B126" s="24"/>
+      <c r="B126" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="22.5">
       <c r="A127" s="1"/>
-      <c r="B127" s="24"/>
+      <c r="B127" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="22.5">
       <c r="A128" s="1"/>
-      <c r="B128" s="24"/>
+      <c r="B128" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="22.5">
       <c r="A129" s="1"/>
-      <c r="B129" s="24"/>
+      <c r="B129" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="22.5">
       <c r="A130" s="1"/>
-      <c r="B130" s="24"/>
+      <c r="B130" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="22.5">
       <c r="A131" s="1"/>
-      <c r="B131" s="24"/>
+      <c r="B131" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="22.5">
       <c r="A132" s="1"/>
-      <c r="B132" s="24"/>
+      <c r="B132" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="22.5">
       <c r="A133" s="1"/>
-      <c r="B133" s="24"/>
+      <c r="B133" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="22.5">
       <c r="A134" s="1"/>
-      <c r="B134" s="24"/>
+      <c r="B134" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="22.5">
       <c r="A135" s="1"/>
-      <c r="B135" s="24"/>
+      <c r="B135" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="22.5">
       <c r="A136" s="1"/>
-      <c r="B136" s="24"/>
+      <c r="B136" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="22.5">
       <c r="A137" s="1"/>
-      <c r="B137" s="24"/>
+      <c r="B137" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="22.5">
       <c r="A138" s="1"/>
-      <c r="B138" s="24"/>
+      <c r="B138" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="22.5">
       <c r="A139" s="1"/>
-      <c r="B139" s="24"/>
+      <c r="B139" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="22.5">
       <c r="A140" s="1"/>
-      <c r="B140" s="24"/>
+      <c r="B140" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="22.5">
       <c r="A141" s="1"/>
-      <c r="B141" s="24"/>
+      <c r="B141" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="22.5">
       <c r="A142" s="1"/>
-      <c r="B142" s="24"/>
+      <c r="B142" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="22.5">
       <c r="A143" s="1"/>
-      <c r="B143" s="24"/>
+      <c r="B143" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="22.5">
       <c r="A144" s="1"/>
-      <c r="B144" s="24"/>
+      <c r="B144" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="22.5">
       <c r="A145" s="1"/>
-      <c r="B145" s="24"/>
+      <c r="B145" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="22.5">
       <c r="A146" s="1"/>
-      <c r="B146" s="24"/>
+      <c r="B146" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="22.5">
       <c r="A147" s="1"/>
-      <c r="B147" s="24"/>
+      <c r="B147" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="22.5">
       <c r="A148" s="1"/>
-      <c r="B148" s="24"/>
+      <c r="B148" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="22.5">
       <c r="A149" s="1"/>
-      <c r="B149" s="24"/>
+      <c r="B149" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="22.5">
       <c r="A150" s="1"/>
-      <c r="B150" s="24"/>
+      <c r="B150" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="22.5">
       <c r="A151" s="1"/>
-      <c r="B151" s="24"/>
+      <c r="B151" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="22.5">
       <c r="A152" s="1"/>
-      <c r="B152" s="24"/>
+      <c r="B152" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="22.5">
       <c r="A153" s="1"/>
-      <c r="B153" s="24"/>
+      <c r="B153" s="25"/>
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="1"/>
@@ -3257,7 +3272,7 @@
       <c r="G2" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="18" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3266,7 +3281,7 @@
       <c r="B3" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D3" s="1" t="s">
@@ -3286,7 +3301,7 @@
       <c r="B4" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D4" s="1" t="s">
@@ -3306,7 +3321,7 @@
       <c r="B5" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D5" s="1" t="s">
@@ -3326,7 +3341,7 @@
       <c r="B6" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D6" s="1" t="s">
@@ -3346,7 +3361,7 @@
       <c r="B7" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D7" s="1" t="s">
@@ -3366,7 +3381,7 @@
       <c r="B8" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D8" s="1" t="s">
@@ -3386,7 +3401,7 @@
       <c r="B9" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D9" s="1" t="s">
@@ -3406,7 +3421,7 @@
       <c r="B10" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D10" s="1" t="s">
@@ -3426,7 +3441,7 @@
       <c r="B11" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D11" s="1" t="s">
@@ -3446,7 +3461,7 @@
       <c r="B12" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D12" s="1" t="s">
@@ -3466,7 +3481,7 @@
       <c r="B13" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D13" s="1" t="s">
@@ -3486,7 +3501,7 @@
       <c r="B14" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D14" s="1" t="s">
@@ -3506,7 +3521,7 @@
       <c r="B15" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D15" s="1" t="s">
@@ -3526,7 +3541,7 @@
       <c r="B16" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D16" s="1" t="s">
@@ -3546,7 +3561,7 @@
       <c r="B17" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D17" s="1" t="s">
@@ -3566,7 +3581,7 @@
       <c r="B18" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D18" s="1" t="s">
@@ -3586,7 +3601,7 @@
       <c r="B19" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D19" s="1" t="s">
@@ -3606,7 +3621,7 @@
       <c r="B20" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D20" s="1" t="s">
@@ -3626,7 +3641,7 @@
       <c r="B21" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D21" s="1" t="s">
@@ -3646,7 +3661,7 @@
       <c r="B22" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D22" s="1" t="s">
@@ -3666,7 +3681,7 @@
       <c r="B23" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D23" s="1" t="s">
@@ -3686,7 +3701,7 @@
       <c r="B24" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D24" s="1" t="s">
@@ -3706,7 +3721,7 @@
       <c r="B25" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D25" s="1" t="s">
@@ -3726,7 +3741,7 @@
       <c r="B26" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D26" s="1" t="s">
@@ -3746,7 +3761,7 @@
       <c r="B27" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D27" s="1" t="s">
@@ -3766,7 +3781,7 @@
       <c r="B28" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D28" s="1" t="s">
@@ -3786,7 +3801,7 @@
       <c r="B29" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D29" s="1" t="s">
@@ -3806,7 +3821,7 @@
       <c r="B30" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D30" s="1" t="s">
@@ -3826,7 +3841,7 @@
       <c r="B31" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D31" s="1" t="s">
@@ -3846,7 +3861,7 @@
       <c r="B32" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D32" s="1" t="s">
@@ -3866,7 +3881,7 @@
       <c r="B33" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D33" s="1" t="s">
@@ -3886,7 +3901,7 @@
       <c r="B34" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D34" s="1" t="s">
@@ -3906,7 +3921,7 @@
       <c r="B35" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D35" s="1" t="s">
@@ -3926,7 +3941,7 @@
       <c r="B36" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C36" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D36" s="1" t="s">
@@ -3946,7 +3961,7 @@
       <c r="B37" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D37" s="1" t="s">
@@ -3966,7 +3981,7 @@
       <c r="B38" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D38" s="1" t="s">
@@ -3986,7 +4001,7 @@
       <c r="B39" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D39" s="1" t="s">
@@ -3999,10 +4014,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="1"/>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="C40" s="18">
+      <c r="C40" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D40" s="1" t="s">
@@ -4018,7 +4033,7 @@
       <c r="B41" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D41" s="1" t="s">
@@ -4034,7 +4049,7 @@
       <c r="B42" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C42" s="18">
+      <c r="C42" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D42" s="1" t="s">
@@ -4050,7 +4065,7 @@
       <c r="B43" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C43" s="18">
+      <c r="C43" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D43" s="1" t="s">
@@ -4066,7 +4081,7 @@
       <c r="B44" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C44" s="18">
+      <c r="C44" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D44" s="1" t="s">
@@ -4079,10 +4094,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="1"/>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D45" s="1" t="s">
@@ -4098,7 +4113,7 @@
       <c r="B46" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C46" s="18">
+      <c r="C46" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D46" s="1" t="s">
@@ -4114,7 +4129,7 @@
       <c r="B47" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C47" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D47" s="1" t="s">
@@ -4130,7 +4145,7 @@
       <c r="B48" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C48" s="18">
+      <c r="C48" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D48" s="1" t="s">
@@ -4146,7 +4161,7 @@
       <c r="B49" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C49" s="18">
+      <c r="C49" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D49" s="1" t="s">
@@ -4162,7 +4177,7 @@
       <c r="B50" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C50" s="18">
+      <c r="C50" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D50" s="1" t="s">
@@ -4178,7 +4193,7 @@
       <c r="B51" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C51" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D51" s="1" t="s">
@@ -4194,7 +4209,7 @@
       <c r="B52" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C52" s="18">
+      <c r="C52" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D52" s="1" t="s">
@@ -4210,7 +4225,7 @@
       <c r="B53" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C53" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D53" s="1" t="s">
@@ -4226,7 +4241,7 @@
       <c r="B54" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C54" s="18">
+      <c r="C54" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D54" s="1" t="s">
@@ -4242,7 +4257,7 @@
       <c r="B55" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C55" s="18">
+      <c r="C55" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D55" s="1" t="s">
@@ -4258,7 +4273,7 @@
       <c r="B56" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C56" s="18">
+      <c r="C56" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D56" s="1" t="s">
@@ -4274,7 +4289,7 @@
       <c r="B57" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C57" s="18">
+      <c r="C57" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D57" s="1" t="s">
@@ -4290,7 +4305,7 @@
       <c r="B58" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C58" s="18">
+      <c r="C58" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D58" s="1" t="s">
@@ -4306,7 +4321,7 @@
       <c r="B59" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C59" s="18">
+      <c r="C59" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D59" s="1" t="s">
@@ -4322,7 +4337,7 @@
       <c r="B60" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C60" s="18">
+      <c r="C60" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D60" s="1" t="s">
@@ -4338,7 +4353,7 @@
       <c r="B61" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C61" s="18">
+      <c r="C61" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D61" s="1" t="s">
@@ -4354,7 +4369,7 @@
       <c r="B62" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C62" s="18">
+      <c r="C62" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D62" s="1" t="s">
@@ -4370,7 +4385,7 @@
       <c r="B63" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C63" s="18">
+      <c r="C63" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D63" s="1" t="s">
@@ -4386,7 +4401,7 @@
       <c r="B64" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C64" s="18">
+      <c r="C64" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D64" s="1" t="s">
@@ -4399,10 +4414,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="1"/>
-      <c r="B65" s="20" t="s">
+      <c r="B65" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="C65" s="18">
+      <c r="C65" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D65" s="1" t="s">
@@ -4418,7 +4433,7 @@
       <c r="B66" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C66" s="18">
+      <c r="C66" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D66" s="1" t="s">
@@ -4434,7 +4449,7 @@
       <c r="B67" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C67" s="18">
+      <c r="C67" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D67" s="1" t="s">
@@ -4450,7 +4465,7 @@
       <c r="B68" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C68" s="18">
+      <c r="C68" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D68" s="1" t="s">
@@ -4466,7 +4481,7 @@
       <c r="B69" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C69" s="18">
+      <c r="C69" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D69" s="1" t="s">
@@ -4482,7 +4497,7 @@
       <c r="B70" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C70" s="18">
+      <c r="C70" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D70" s="1" t="s">
@@ -4498,7 +4513,7 @@
       <c r="B71" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="C71" s="18">
+      <c r="C71" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D71" s="1" t="s">
@@ -4514,7 +4529,7 @@
       <c r="B72" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C72" s="18">
+      <c r="C72" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D72" s="1" t="s">
@@ -4530,7 +4545,7 @@
       <c r="B73" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C73" s="18">
+      <c r="C73" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D73" s="1" t="s">
@@ -4546,7 +4561,7 @@
       <c r="B74" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C74" s="18">
+      <c r="C74" s="19">
         <f>PROPER(Tableau1[[#This Row], [Colonne1]])</f>
       </c>
       <c r="D74" s="1" t="s">

</xml_diff>